<commit_message>
database dan UI dashboard
</commit_message>
<xml_diff>
--- a/riwayat-skrining-2025-12-19_21-18.xlsx
+++ b/riwayat-skrining-2025-12-19_21-18.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oslan\Documents\CodeIgniter\tensitrack\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A54BBA-A792-4D42-9A11-7D9533E4E2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="188">
   <si>
     <t>No</t>
   </si>
@@ -63,7 +47,7 @@
     <t>Faktor Risiko Terpilih</t>
   </si>
   <si>
-    <t>Hasil Risiko</t>
+    <t>Email</t>
   </si>
   <si>
     <t>13/12/2025 13:24</t>
@@ -84,7 +68,7 @@
 4. Mudah marah atau ketidakstabilan emosional</t>
   </si>
   <si>
-    <t>Risiko hipertensi sedang</t>
+    <t>gamingplay56@gmail.com</t>
   </si>
   <si>
     <t>11/12/2025 09:18</t>
@@ -99,6 +83,9 @@
     <t>1. Riwayat hipertensi pada keluarga inti
 2. Stres &amp; cemas berlebih
 3. Pola Tidur Buruk / Begadang</t>
+  </si>
+  <si>
+    <t>alvin.122320017@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 12:41</t>
@@ -117,6 +104,9 @@
 2. Stres &amp; cemas berlebih
 3. Pola Tidur Buruk / Begadang
 4. Mudah marah atau ketidakstabilan emosional</t>
+  </si>
+  <si>
+    <t>yasminzka691@gmail.com</t>
   </si>
   <si>
     <t>Made Natalia Wati</t>
@@ -132,7 +122,7 @@
 5. Tekanan darah meningkat (121-139 / 81-89 mmHg)</t>
   </si>
   <si>
-    <t>Risiko hipertensi tinggi</t>
+    <t>brysonzoe25@gmail.con</t>
   </si>
   <si>
     <t>Michelle Ivana Adelin</t>
@@ -142,6 +132,9 @@
 2. Pola Tidur Buruk / Begadang
 3. Tekanan darah meningkat (121-139 / 81-89 mmHg)
 4. Obesitas (IMT ≥ 25)</t>
+  </si>
+  <si>
+    <t>michelle.123130066@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 12:40</t>
@@ -160,6 +153,9 @@
 5. Mudah marah atau ketidakstabilan emosional</t>
   </si>
   <si>
+    <t>muhammad.122380089@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>09/12/2025 12:23</t>
   </si>
   <si>
@@ -170,6 +166,9 @@
 2. Stres &amp; cemas berlebih
 3. Pola Tidur Buruk / Begadang
 4. Mudah marah atau ketidakstabilan emosional</t>
+  </si>
+  <si>
+    <t>akhmad.123430096@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 12:19</t>
@@ -183,6 +182,9 @@
 3. Stres &amp; cemas berlebih
 4. Pola Tidur Buruk / Begadang
 5. Perokok pasif</t>
+  </si>
+  <si>
+    <t>faiz.125430048@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 12:10</t>
@@ -204,6 +206,9 @@
 8. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>nubaiddiyar952@gmail.com</t>
+  </si>
+  <si>
     <t>09/12/2025 11:52</t>
   </si>
   <si>
@@ -219,6 +224,9 @@
 7. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>pingki.125330060@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>09/12/2025 11:51</t>
   </si>
   <si>
@@ -231,6 +239,9 @@
 4. Perokok pasif
 5. Mudah marah atau ketidakstabilan emosional
 6. Obesitas (IMT ≥ 25)</t>
+  </si>
+  <si>
+    <t>nadia.125330083@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 11:31</t>
@@ -249,6 +260,9 @@
 8. Mudah marah atau ketidakstabilan emosional</t>
   </si>
   <si>
+    <t>bintang.123430028@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>09/12/2025 11:01</t>
   </si>
   <si>
@@ -263,6 +277,9 @@
 6. Tekanan darah meningkat (121-139 / 81-89 mmHg)</t>
   </si>
   <si>
+    <t>ilham.121430011@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>09/12/2025 10:58</t>
   </si>
   <si>
@@ -277,6 +294,9 @@
 6. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>petrasitompul1@gmail.com</t>
+  </si>
+  <si>
     <t>09/12/2025 10:51</t>
   </si>
   <si>
@@ -288,6 +308,9 @@
 3. Pola Tidur Buruk / Begadang
 4. Tekanan darah meningkat (121-139 / 81-89 mmHg)
 5. Obesitas (IMT ≥ 25)</t>
+  </si>
+  <si>
+    <t>fajar.121430154@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 10:47</t>
@@ -307,6 +330,9 @@
 6. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>ramziakmal23@gmail.com</t>
+  </si>
+  <si>
     <t>09/12/2025 10:39</t>
   </si>
   <si>
@@ -316,6 +342,17 @@
     <t>110/80</t>
   </si>
   <si>
+    <t>1. Riwayat hipertensi pada keluarga inti
+2. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
+3. Stres &amp; cemas berlebih
+4. Pola Tidur Buruk / Begadang
+5. Perokok pasif
+7. Obesitas (IMT ≥ 25)</t>
+  </si>
+  <si>
+    <t>sariahta407@gmail.com</t>
+  </si>
+  <si>
     <t>09/12/2025 10:22</t>
   </si>
   <si>
@@ -325,10 +362,27 @@
     <t>100/80</t>
   </si>
   <si>
+    <t>1. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
+2. Pola Tidur Buruk / Begadang</t>
+  </si>
+  <si>
+    <t>aulia.125320011@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>09/12/2025 10:20</t>
   </si>
   <si>
     <t>Siti Nur Kholilah</t>
+  </si>
+  <si>
+    <t>1. Riwayat hipertensi pada keluarga inti
+2. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
+3. Stres &amp; cemas berlebih
+4. Pola Tidur Buruk / Begadang
+6. Obesitas (IMT ≥ 25)</t>
+  </si>
+  <si>
+    <t>siti.125320029@student.itera.ac.id</t>
   </si>
   <si>
     <t>09/12/2025 09:48</t>
@@ -343,6 +397,9 @@
 4. Stres &amp; cemas berlebih
 5. Pola Tidur Buruk / Begadang
 6. Perokok pasif</t>
+  </si>
+  <si>
+    <t>muhammad.124430084@student.itera.ac.id</t>
   </si>
   <si>
     <t>08/12/2025 15:25</t>
@@ -360,6 +417,9 @@
 7. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>ghyna.123410032@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>Nadia Shakila Hendri</t>
   </si>
   <si>
@@ -371,6 +431,9 @@
 6. Mudah marah atau ketidakstabilan emosional</t>
   </si>
   <si>
+    <t>nadia.123410037@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>08/12/2025 14:45</t>
   </si>
   <si>
@@ -378,6 +441,9 @@
   </si>
   <si>
     <t>140/90</t>
+  </si>
+  <si>
+    <t>ratireiza8020@gmail.com</t>
   </si>
   <si>
     <t>08/12/2025 14:44</t>
@@ -393,6 +459,9 @@
 5. Mudah marah atau ketidakstabilan emosional</t>
   </si>
   <si>
+    <t>peggy.122430109@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>Anisa Prasetya Putri Kartini</t>
   </si>
   <si>
@@ -403,6 +472,9 @@
 5. Perokok pasif</t>
   </si>
   <si>
+    <t>nisaprsetya.4@gmail.com</t>
+  </si>
+  <si>
     <t>08/12/2025 14:37</t>
   </si>
   <si>
@@ -412,7 +484,7 @@
     <t>1. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu</t>
   </si>
   <si>
-    <t>Risiko hipertensi rendah</t>
+    <t>junisa.122190028@student.itera.ac.id</t>
   </si>
   <si>
     <t>08/12/2025 14:36</t>
@@ -422,6 +494,9 @@
   </si>
   <si>
     <t>100/90</t>
+  </si>
+  <si>
+    <t>yuridelfita02@gmail.com</t>
   </si>
   <si>
     <t>08/12/2025 14:28</t>
@@ -438,12 +513,18 @@
 6. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>rizky.122470036@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>08/12/2025 11:40</t>
   </si>
   <si>
     <t>Ratu Sabela Rizkika</t>
   </si>
   <si>
+    <t>ratusabelarizkika1311@gmail.com</t>
+  </si>
+  <si>
     <t>08/12/2025 11:39</t>
   </si>
   <si>
@@ -451,6 +532,9 @@
   </si>
   <si>
     <t>130/90</t>
+  </si>
+  <si>
+    <t>zahra@email.com</t>
   </si>
   <si>
     <t>08/12/2025 11:31</t>
@@ -463,13 +547,22 @@
 2. Perokok pasif</t>
   </si>
   <si>
+    <t>chelsita.125290010@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>08/12/2025 11:30</t>
   </si>
   <si>
     <t>Aniq Muflihah</t>
   </si>
   <si>
+    <t>aniq.125290052@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>Putra Dermawan Lumban Batu</t>
+  </si>
+  <si>
+    <t>putra.125480075@student.itera.ac.id</t>
   </si>
   <si>
     <t>08/12/2025 11:29</t>
@@ -486,6 +579,9 @@
 3. Pola Tidur Buruk / Begadang</t>
   </si>
   <si>
+    <t>jasmine.125290011@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>Dimas Hadi Prasetiyo</t>
   </si>
   <si>
@@ -493,11 +589,17 @@
 2. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu</t>
   </si>
   <si>
+    <t>dimas.125480047@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>Jona Christian tamba</t>
   </si>
   <si>
     <t>1. Pola Tidur Buruk / Begadang
 2. Perokok pasif</t>
+  </si>
+  <si>
+    <t>jona.125480019@student.itera.ac.id</t>
   </si>
   <si>
     <t>08/12/2025 11:12</t>
@@ -515,6 +617,9 @@
 7. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>oslandpurba262@gmail.com</t>
+  </si>
+  <si>
     <t>08/12/2025 10:36</t>
   </si>
   <si>
@@ -530,14 +635,16 @@
 4. Pola Tidur Buruk / Begadang</t>
   </si>
   <si>
+    <t>claudia.125270082@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>VERONIKA BR SIBARANI</t>
   </si>
   <si>
     <t>121/88</t>
   </si>
   <si>
-    <t>1. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
-2. Pola Tidur Buruk / Begadang</t>
+    <t>veronika.125110028@student.itera.ac.id</t>
   </si>
   <si>
     <t>08/12/2025 10:34</t>
@@ -557,6 +664,9 @@
 6. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
+    <t>viona.125270001@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>08/12/2025 10:32</t>
   </si>
   <si>
@@ -570,6 +680,9 @@
 2. Pola Tidur Buruk / Begadang</t>
   </si>
   <si>
+    <t>alif.125480085@student.itera.ac.id</t>
+  </si>
+  <si>
     <t>08/12/2025 10:29</t>
   </si>
   <si>
@@ -577,6 +690,9 @@
   </si>
   <si>
     <t>112/64</t>
+  </si>
+  <si>
+    <t>ilhamsuhada486@gmail.com</t>
   </si>
   <si>
     <t>08/12/2025 10:27</t>
@@ -595,33 +711,29 @@
 5. Obesitas (IMT ≥ 25)</t>
   </si>
   <si>
-    <t>1. Riwayat hipertensi pada keluarga inti
-2. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
-3. Stres &amp; cemas berlebih
-4. Pola Tidur Buruk / Begadang
-5. Perokok pasif
-7. Obesitas (IMT ≥ 25)</t>
-  </si>
-  <si>
-    <t>1. Riwayat hipertensi pada keluarga inti
-2. Konsumsi Tinggi Garam (Asin) &amp; Berbumbu
-3. Stres &amp; cemas berlebih
-4. Pola Tidur Buruk / Begadang
-6. Obesitas (IMT ≥ 25)</t>
+    <t>elisabeth.122430104@student.itera.ac.id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -648,33 +760,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -964,29 +1068,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A18">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="true" style="2"/>
+    <col min="2" max="2" width="20" customWidth="true" style="2"/>
+    <col min="3" max="3" width="37.6640625" customWidth="true" style="2"/>
+    <col min="4" max="4" width="16.44140625" customWidth="true" style="2"/>
+    <col min="5" max="5" width="11.6640625" customWidth="true" style="2"/>
+    <col min="6" max="6" width="14" customWidth="true" style="2"/>
+    <col min="7" max="7" width="12.88671875" customWidth="true" style="2"/>
+    <col min="8" max="8" width="5.88671875" customWidth="true" style="2"/>
+    <col min="9" max="9" width="15.33203125" customWidth="true" style="2"/>
+    <col min="10" max="10" width="58.88671875" customWidth="true" style="4"/>
+    <col min="11" max="11" width="29.44140625" customWidth="true" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" customHeight="1" ht="57.6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1056,7 +1163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" customHeight="1" ht="43.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1088,21 +1195,21 @@
         <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" customHeight="1" ht="57.6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
         <v>22</v>
@@ -1117,27 +1224,27 @@
         <v>21.3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" customHeight="1" ht="72">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>20</v>
@@ -1152,27 +1259,27 @@
         <v>22.7</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" customHeight="1" ht="57.6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>20</v>
@@ -1187,24 +1294,24 @@
         <v>27.1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" customHeight="1" ht="72">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -1222,24 +1329,24 @@
         <v>20.8</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" customHeight="1" ht="57.6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -1254,27 +1361,27 @@
         <v>56</v>
       </c>
       <c r="H8" s="2">
-        <v>19.399999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" customHeight="1" ht="72">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -1295,21 +1402,21 @@
         <v>14</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" customHeight="1" ht="115.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
@@ -1327,27 +1434,27 @@
         <v>28.1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" customHeight="1" ht="100.8">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2">
         <v>18</v>
@@ -1362,27 +1469,27 @@
         <v>25.3</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" customHeight="1" ht="86.4">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2">
         <v>17</v>
@@ -1397,24 +1504,24 @@
         <v>25.2</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" customHeight="1" ht="115.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
@@ -1435,21 +1542,21 @@
         <v>14</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" customHeight="1" ht="86.4">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -1467,24 +1574,24 @@
         <v>25</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" customHeight="1" ht="86.4">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
@@ -1502,24 +1609,24 @@
         <v>26.9</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" customHeight="1" ht="72">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
@@ -1537,24 +1644,24 @@
         <v>30</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" customHeight="1" ht="86.4">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>13</v>
@@ -1572,27 +1679,27 @@
         <v>28.2</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" customHeight="1" ht="86.4">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2">
         <v>22</v>
@@ -1607,24 +1714,24 @@
         <v>34.6</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" customHeight="1" ht="28.8">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -1639,30 +1746,30 @@
         <v>36</v>
       </c>
       <c r="H19" s="2">
-        <v>16.399999999999999</v>
+        <v>16.4</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" customHeight="1" ht="72">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2">
         <v>18</v>
@@ -1677,24 +1784,24 @@
         <v>26.3</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" customHeight="1" ht="86.4">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -1715,24 +1822,24 @@
         <v>14</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" customHeight="1" ht="100.8">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2">
         <v>21</v>
@@ -1747,27 +1854,27 @@
         <v>25.2</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" customHeight="1" ht="86.4">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2">
         <v>21</v>
@@ -1779,30 +1886,30 @@
         <v>46</v>
       </c>
       <c r="H23" s="2">
-        <v>18.899999999999999</v>
+        <v>18.9</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" customHeight="1" ht="86.4">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="2">
         <v>21</v>
@@ -1817,27 +1924,27 @@
         <v>21.5</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" customHeight="1" ht="72">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2">
         <v>21</v>
@@ -1852,27 +1959,27 @@
         <v>23.1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" customHeight="1" ht="72">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="2">
         <v>22</v>
@@ -1887,27 +1994,27 @@
         <v>14.8</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E27" s="2">
         <v>21</v>
@@ -1922,27 +2029,27 @@
         <v>17.7</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" customHeight="1" ht="72">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="2">
         <v>21</v>
@@ -1957,24 +2064,24 @@
         <v>16.8</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" customHeight="1" ht="86.4">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>13</v>
@@ -1992,24 +2099,24 @@
         <v>27.8</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" customHeight="1" ht="43.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>13</v>
@@ -2024,30 +2131,30 @@
         <v>51</v>
       </c>
       <c r="H30" s="2">
-        <v>17.899999999999999</v>
+        <v>17.9</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" customHeight="1" ht="72">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2">
         <v>23</v>
@@ -2062,27 +2169,27 @@
         <v>24</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" customHeight="1" ht="28.8">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2">
         <v>18</v>
@@ -2100,24 +2207,24 @@
         <v>14</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E33" s="2">
         <v>18</v>
@@ -2135,21 +2242,21 @@
         <v>14</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" customHeight="1" ht="72">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>13</v>
@@ -2167,27 +2274,27 @@
         <v>18</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" customHeight="1" ht="43.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E35" s="2">
         <v>19</v>
@@ -2199,27 +2306,27 @@
         <v>49</v>
       </c>
       <c r="H35" s="2">
-        <v>19.899999999999999</v>
+        <v>19.9</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" customHeight="1" ht="28.8">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>13</v>
@@ -2237,24 +2344,24 @@
         <v>24.2</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" customHeight="1" ht="28.8">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>13</v>
@@ -2275,21 +2382,21 @@
         <v>14</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" customHeight="1" ht="100.8">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>13</v>
@@ -2307,27 +2414,27 @@
         <v>27.1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" customHeight="1" ht="57.6">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="2">
         <v>18</v>
@@ -2339,30 +2446,30 @@
         <v>51</v>
       </c>
       <c r="H39" s="2">
-        <v>20.399999999999999</v>
+        <v>20.4</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" customHeight="1" ht="28.8">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" s="2">
         <v>18</v>
@@ -2377,27 +2484,27 @@
         <v>19</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" customHeight="1" ht="86.4">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E41" s="2">
         <v>17</v>
@@ -2412,24 +2519,24 @@
         <v>28.4</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" customHeight="1" ht="28.8">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>13</v>
@@ -2447,24 +2554,24 @@
         <v>24.7</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" customHeight="1" ht="72">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>13</v>
@@ -2479,30 +2586,30 @@
         <v>49</v>
       </c>
       <c r="H43" s="2">
-        <v>18.899999999999999</v>
+        <v>18.9</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" customHeight="1" ht="72">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E44" s="2">
         <v>20</v>
@@ -2517,16 +2624,27 @@
         <v>25.5</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>29</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>